<commit_message>
profit calculation step 3
</commit_message>
<xml_diff>
--- a/results_step3_zonal.xlsx
+++ b/results_step3_zonal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6601c3f8e6edde6a/Documents/Ms_Sustainable_Energy/46755_Renewables_in_electricity_markets/REIM_Github/RenewablesInElectricityMarkets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="115_{AAA1D341-523E-49BC-B362-3882824E717D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86EF6968-ECA6-431F-B32B-519F41795441}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="115_{C15E41B9-484D-4BA6-B050-78D856857939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9E935991-AE02-42CD-AA08-782EB1BDAFFB}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" firstSheet="6" activeTab="12" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" firstSheet="11" activeTab="12" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
   </bookViews>
   <sheets>
     <sheet name="DA_Prices" sheetId="1" r:id="rId1"/>
@@ -123,18 +123,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -149,9 +143,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -465,297 +460,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C885426-E243-4707-84A6-86E79A0CB291}">
-  <dimension ref="A1:C25"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>10.52</v>
-      </c>
-      <c r="B2">
-        <v>10.52</v>
-      </c>
-      <c r="C2">
-        <v>10.52</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>10.52</v>
-      </c>
-      <c r="B3">
-        <v>10.52</v>
-      </c>
-      <c r="C3">
-        <v>10.52</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>10</v>
-      </c>
-      <c r="B4">
-        <v>10</v>
-      </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>10.52</v>
-      </c>
-      <c r="B5">
-        <v>10.52</v>
-      </c>
-      <c r="C5">
-        <v>10.52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>10</v>
-      </c>
-      <c r="B6">
-        <v>10</v>
-      </c>
-      <c r="C6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>10</v>
-      </c>
-      <c r="B7">
-        <v>10</v>
-      </c>
-      <c r="C7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>10.52</v>
-      </c>
-      <c r="B8">
-        <v>10.52</v>
-      </c>
-      <c r="C8">
-        <v>10.52</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>10.52</v>
-      </c>
-      <c r="B9">
-        <v>10.52</v>
-      </c>
-      <c r="C9">
-        <v>10.52</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>10.52</v>
-      </c>
-      <c r="B10">
-        <v>10.52</v>
-      </c>
-      <c r="C10">
-        <v>10.52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>10.52</v>
-      </c>
-      <c r="B11">
-        <v>10.52</v>
-      </c>
-      <c r="C11">
-        <v>10.52</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>10.52</v>
-      </c>
-      <c r="B12">
-        <v>10.52</v>
-      </c>
-      <c r="C12">
-        <v>10.52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>10.52</v>
-      </c>
-      <c r="B13">
-        <v>10.52</v>
-      </c>
-      <c r="C13">
-        <v>10.52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <v>10.89</v>
-      </c>
-      <c r="B14">
-        <v>10.89</v>
-      </c>
-      <c r="C14">
-        <v>10.89</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <v>10.89</v>
-      </c>
-      <c r="B15">
-        <v>10.89</v>
-      </c>
-      <c r="C15">
-        <v>10.89</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <v>10.52</v>
-      </c>
-      <c r="B16">
-        <v>10.52</v>
-      </c>
-      <c r="C16">
-        <v>10.52</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <v>10.52</v>
-      </c>
-      <c r="B17">
-        <v>10.52</v>
-      </c>
-      <c r="C17">
-        <v>10.52</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18">
-        <v>10.52</v>
-      </c>
-      <c r="B18">
-        <v>10.52</v>
-      </c>
-      <c r="C18">
-        <v>10.52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19">
-        <v>10.52</v>
-      </c>
-      <c r="B19">
-        <v>10.52</v>
-      </c>
-      <c r="C19">
-        <v>10.52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A20">
-        <v>10.89</v>
-      </c>
-      <c r="B20">
-        <v>10.89</v>
-      </c>
-      <c r="C20">
-        <v>10.89</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A21">
-        <v>10.89</v>
-      </c>
-      <c r="B21">
-        <v>10.89</v>
-      </c>
-      <c r="C21">
-        <v>10.89</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22">
-        <v>10.52</v>
-      </c>
-      <c r="B22">
-        <v>10.52</v>
-      </c>
-      <c r="C22">
-        <v>10.52</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23">
-        <v>10.52</v>
-      </c>
-      <c r="B23">
-        <v>10.52</v>
-      </c>
-      <c r="C23">
-        <v>10.52</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24">
-        <v>10.52</v>
-      </c>
-      <c r="B24">
-        <v>10.52</v>
-      </c>
-      <c r="C24">
-        <v>10.52</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25">
-        <v>10</v>
-      </c>
-      <c r="B25">
-        <v>10</v>
-      </c>
-      <c r="C25">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D559A612-A82F-4CEB-B5FF-C3D8A0046DF4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5C711D90-52B5-4570-A517-FF5BF700D938}">
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -775,266 +480,266 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>541.62</v>
+        <v>10.52</v>
       </c>
       <c r="B2">
-        <v>310.78000000000003</v>
+        <v>10.52</v>
       </c>
       <c r="C2">
-        <v>390.69</v>
+        <v>10.52</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
-        <v>890.00999999999988</v>
+        <v>10.52</v>
       </c>
       <c r="B3">
-        <v>247.14</v>
+        <v>10.52</v>
       </c>
       <c r="C3">
-        <v>153.62</v>
+        <v>10.52</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
-        <v>661.56</v>
+        <v>10</v>
       </c>
       <c r="B4">
-        <v>235.36999999999998</v>
+        <v>10</v>
       </c>
       <c r="C4">
-        <v>241.72000000000003</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
-        <v>550.45000000000005</v>
+        <v>10.52</v>
       </c>
       <c r="B5">
-        <v>386.25</v>
+        <v>10.52</v>
       </c>
       <c r="C5">
-        <v>344.03999999999996</v>
+        <v>10.52</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
-        <v>688.06000000000006</v>
+        <v>10</v>
       </c>
       <c r="B6">
-        <v>248.64</v>
+        <v>10</v>
       </c>
       <c r="C6">
-        <v>250.21</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>559.78</v>
+        <v>10</v>
       </c>
       <c r="B7">
-        <v>338.74</v>
+        <v>10</v>
       </c>
       <c r="C7">
-        <v>241.72000000000003</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
-        <v>794.35</v>
+        <v>10.52</v>
       </c>
       <c r="B8">
-        <v>241.25</v>
+        <v>10.52</v>
       </c>
       <c r="C8">
-        <v>313.82</v>
+        <v>10.52</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>1135.1499999999999</v>
+        <v>10.52</v>
       </c>
       <c r="B9">
-        <v>485.53000000000003</v>
+        <v>10.52</v>
       </c>
       <c r="C9">
-        <v>364.7</v>
+        <v>10.52</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
-        <v>1180.9299999999998</v>
+        <v>10.52</v>
       </c>
       <c r="B10">
-        <v>224.10000000000002</v>
+        <v>10.52</v>
       </c>
       <c r="C10">
-        <v>553.95000000000005</v>
+        <v>10.52</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>1356.2099999999998</v>
+        <v>10.52</v>
       </c>
       <c r="B11">
-        <v>468.17999999999995</v>
+        <v>10.52</v>
       </c>
       <c r="C11">
-        <v>295.16000000000003</v>
+        <v>10.52</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
-        <v>664.11</v>
+        <v>10.52</v>
       </c>
       <c r="B12">
-        <v>473.27</v>
+        <v>10.52</v>
       </c>
       <c r="C12">
-        <v>559.79</v>
+        <v>10.52</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
-        <v>1062.58</v>
+        <v>10.52</v>
       </c>
       <c r="B13">
-        <v>493.52</v>
+        <v>10.52</v>
       </c>
       <c r="C13">
-        <v>443.15999999999997</v>
+        <v>10.52</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
-        <v>1047.48</v>
+        <v>10.89</v>
       </c>
       <c r="B14">
-        <v>621.93999999999994</v>
+        <v>10.89</v>
       </c>
       <c r="C14">
-        <v>553.95000000000005</v>
+        <v>10.89</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>1107.9100000000001</v>
+        <v>10.89</v>
       </c>
       <c r="B15">
-        <v>536.32999999999993</v>
+        <v>10.89</v>
       </c>
       <c r="C15">
-        <v>553.95000000000005</v>
+        <v>10.89</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
-        <v>1084.58</v>
+        <v>10.52</v>
       </c>
       <c r="B16">
-        <v>389.46000000000004</v>
+        <v>10.52</v>
       </c>
       <c r="C16">
-        <v>433.84000000000003</v>
+        <v>10.52</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
-        <v>939.15</v>
+        <v>10.52</v>
       </c>
       <c r="B17">
-        <v>303.19</v>
+        <v>10.52</v>
       </c>
       <c r="C17">
-        <v>542.29999999999995</v>
+        <v>10.52</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
-        <v>1062.72</v>
+        <v>10.52</v>
       </c>
       <c r="B18">
-        <v>482.81</v>
+        <v>10.52</v>
       </c>
       <c r="C18">
-        <v>577.28</v>
+        <v>10.52</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A19">
-        <v>893.21999999999991</v>
+        <v>10.52</v>
       </c>
       <c r="B19">
-        <v>402.87</v>
+        <v>10.52</v>
       </c>
       <c r="C19">
-        <v>402.87</v>
+        <v>10.52</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A20">
-        <v>1319.9500000000003</v>
+        <v>10.89</v>
       </c>
       <c r="B20">
-        <v>564.54999999999995</v>
+        <v>10.89</v>
       </c>
       <c r="C20">
-        <v>455.88</v>
+        <v>10.89</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A21">
-        <v>1267.1499999999999</v>
+        <v>10.89</v>
       </c>
       <c r="B21">
-        <v>628.48</v>
+        <v>10.89</v>
       </c>
       <c r="C21">
-        <v>386.77</v>
+        <v>10.89</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22">
-        <v>1017.85</v>
+        <v>10.52</v>
       </c>
       <c r="B22">
-        <v>535.45000000000005</v>
+        <v>10.52</v>
       </c>
       <c r="C22">
-        <v>366.62</v>
+        <v>10.52</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23">
-        <v>1172.55</v>
+        <v>10.52</v>
       </c>
       <c r="B23">
-        <v>543.38</v>
+        <v>10.52</v>
       </c>
       <c r="C23">
-        <v>255.19</v>
+        <v>10.52</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24">
-        <v>1031.28</v>
+        <v>10.52</v>
       </c>
       <c r="B24">
-        <v>477.92000000000007</v>
+        <v>10.52</v>
       </c>
       <c r="C24">
-        <v>340.53</v>
+        <v>10.52</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A25">
-        <v>611.15</v>
+        <v>10</v>
       </c>
       <c r="B25">
-        <v>412.45000000000005</v>
+        <v>10</v>
       </c>
       <c r="C25">
-        <v>153.62</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1042,8 +747,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2700EE2D-15D3-4838-8850-845370C60D7C}">
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A12C7603-5253-47D3-847A-E00A72665BC8}">
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1063,6 +768,294 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
+        <v>541.62</v>
+      </c>
+      <c r="B2">
+        <v>310.78000000000003</v>
+      </c>
+      <c r="C2">
+        <v>390.69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>890.00999999999988</v>
+      </c>
+      <c r="B3">
+        <v>247.14</v>
+      </c>
+      <c r="C3">
+        <v>153.62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>661.56</v>
+      </c>
+      <c r="B4">
+        <v>235.36999999999998</v>
+      </c>
+      <c r="C4">
+        <v>241.72000000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>550.45000000000005</v>
+      </c>
+      <c r="B5">
+        <v>386.25</v>
+      </c>
+      <c r="C5">
+        <v>344.03999999999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>688.06000000000006</v>
+      </c>
+      <c r="B6">
+        <v>248.64</v>
+      </c>
+      <c r="C6">
+        <v>250.21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>559.78</v>
+      </c>
+      <c r="B7">
+        <v>338.74</v>
+      </c>
+      <c r="C7">
+        <v>241.72000000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>794.35</v>
+      </c>
+      <c r="B8">
+        <v>241.25</v>
+      </c>
+      <c r="C8">
+        <v>313.82</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>1135.1499999999999</v>
+      </c>
+      <c r="B9">
+        <v>485.53000000000003</v>
+      </c>
+      <c r="C9">
+        <v>364.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>1180.9299999999998</v>
+      </c>
+      <c r="B10">
+        <v>224.10000000000002</v>
+      </c>
+      <c r="C10">
+        <v>553.95000000000005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>1356.2099999999998</v>
+      </c>
+      <c r="B11">
+        <v>468.17999999999995</v>
+      </c>
+      <c r="C11">
+        <v>295.16000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>664.11</v>
+      </c>
+      <c r="B12">
+        <v>473.27</v>
+      </c>
+      <c r="C12">
+        <v>559.79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>1062.58</v>
+      </c>
+      <c r="B13">
+        <v>493.52</v>
+      </c>
+      <c r="C13">
+        <v>443.15999999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>1047.48</v>
+      </c>
+      <c r="B14">
+        <v>621.93999999999994</v>
+      </c>
+      <c r="C14">
+        <v>553.95000000000005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>1107.9100000000001</v>
+      </c>
+      <c r="B15">
+        <v>536.32999999999993</v>
+      </c>
+      <c r="C15">
+        <v>553.95000000000005</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>1084.58</v>
+      </c>
+      <c r="B16">
+        <v>389.46000000000004</v>
+      </c>
+      <c r="C16">
+        <v>433.84000000000003</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>939.15</v>
+      </c>
+      <c r="B17">
+        <v>303.19</v>
+      </c>
+      <c r="C17">
+        <v>542.29999999999995</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>1062.72</v>
+      </c>
+      <c r="B18">
+        <v>482.81</v>
+      </c>
+      <c r="C18">
+        <v>577.28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>893.21999999999991</v>
+      </c>
+      <c r="B19">
+        <v>402.87</v>
+      </c>
+      <c r="C19">
+        <v>402.87</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>1319.9500000000003</v>
+      </c>
+      <c r="B20">
+        <v>564.54999999999995</v>
+      </c>
+      <c r="C20">
+        <v>455.88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>1267.1499999999999</v>
+      </c>
+      <c r="B21">
+        <v>628.48</v>
+      </c>
+      <c r="C21">
+        <v>386.77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>1017.85</v>
+      </c>
+      <c r="B22">
+        <v>535.45000000000005</v>
+      </c>
+      <c r="C22">
+        <v>366.62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>1172.55</v>
+      </c>
+      <c r="B23">
+        <v>543.38</v>
+      </c>
+      <c r="C23">
+        <v>255.19</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>1031.28</v>
+      </c>
+      <c r="B24">
+        <v>477.92000000000007</v>
+      </c>
+      <c r="C24">
+        <v>340.53</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>611.15</v>
+      </c>
+      <c r="B25">
+        <v>412.45000000000005</v>
+      </c>
+      <c r="C25">
+        <v>153.62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{394DCE47-7421-4E28-B981-D3DAF51773C5}">
+  <dimension ref="A1:C25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2">
         <v>48.813710260000001</v>
       </c>
       <c r="B2">
@@ -1331,16 +1324,16 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{93008EC9-18E2-402E-A6A1-78C91AB7F316}">
-  <dimension ref="A1:L27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{060B79CC-9028-47CB-A1F5-658D20F5FC76}">
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -1378,984 +1371,165 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>1800</v>
-      </c>
-      <c r="I2">
-        <v>2020</v>
-      </c>
-      <c r="J2">
-        <v>156</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0</v>
+      </c>
+      <c r="F2" s="1">
+        <v>229.40000000000055</v>
+      </c>
+      <c r="G2" s="1">
+        <v>229.40000000000055</v>
+      </c>
+      <c r="H2" s="1">
+        <v>42960</v>
+      </c>
+      <c r="I2" s="1">
+        <v>48240</v>
+      </c>
+      <c r="J2" s="1">
+        <v>3564</v>
+      </c>
+      <c r="K2" s="1">
+        <v>458.80000000000109</v>
+      </c>
+      <c r="L2" s="1">
         <v>-14.800000000000068</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>1800</v>
-      </c>
-      <c r="I3">
-        <v>2020</v>
-      </c>
-      <c r="J3">
-        <v>156</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>1592</v>
-      </c>
-      <c r="I4">
-        <v>1812</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>0</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>1800</v>
-      </c>
-      <c r="I5">
-        <v>2020</v>
-      </c>
-      <c r="J5">
-        <v>156</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>1592</v>
-      </c>
-      <c r="I6">
-        <v>1812</v>
-      </c>
-      <c r="J6">
-        <v>0</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>0</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>1592</v>
-      </c>
-      <c r="I7">
-        <v>1812</v>
-      </c>
-      <c r="J7">
-        <v>0</v>
-      </c>
-      <c r="K7">
-        <v>0</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>0</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>1800</v>
-      </c>
-      <c r="I8">
-        <v>2020</v>
-      </c>
-      <c r="J8">
-        <v>156</v>
-      </c>
-      <c r="K8">
-        <v>0</v>
-      </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>0</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>1800</v>
-      </c>
-      <c r="I9">
-        <v>2020</v>
-      </c>
-      <c r="J9">
-        <v>156</v>
-      </c>
-      <c r="K9">
-        <v>0</v>
-      </c>
-      <c r="L9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>0</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10">
-        <v>0</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>0</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>1800</v>
-      </c>
-      <c r="I10">
-        <v>2020</v>
-      </c>
-      <c r="J10">
-        <v>156</v>
-      </c>
-      <c r="K10">
-        <v>0</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>0</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>1800</v>
-      </c>
-      <c r="I11">
-        <v>2020</v>
-      </c>
-      <c r="J11">
-        <v>156</v>
-      </c>
-      <c r="K11">
-        <v>0</v>
-      </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>0</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>1800</v>
-      </c>
-      <c r="I12">
-        <v>2020</v>
-      </c>
-      <c r="J12">
-        <v>156</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>0</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>1800</v>
-      </c>
-      <c r="I13">
-        <v>2020</v>
-      </c>
-      <c r="J13">
-        <v>156</v>
-      </c>
-      <c r="K13">
-        <v>0</v>
-      </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <v>0</v>
-      </c>
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>57.350000000000136</v>
-      </c>
-      <c r="G14">
-        <v>57.350000000000136</v>
-      </c>
-      <c r="H14">
-        <v>1948</v>
-      </c>
-      <c r="I14">
-        <v>2168</v>
-      </c>
-      <c r="J14">
-        <v>267</v>
-      </c>
-      <c r="K14">
-        <v>114.70000000000027</v>
-      </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <v>0</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>57.350000000000136</v>
-      </c>
-      <c r="G15">
-        <v>57.350000000000136</v>
-      </c>
-      <c r="H15">
-        <v>1948</v>
-      </c>
-      <c r="I15">
-        <v>2168</v>
-      </c>
-      <c r="J15">
-        <v>267</v>
-      </c>
-      <c r="K15">
-        <v>114.70000000000027</v>
-      </c>
-      <c r="L15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <v>0</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <v>1800</v>
-      </c>
-      <c r="I16">
-        <v>2020</v>
-      </c>
-      <c r="J16">
-        <v>156</v>
-      </c>
-      <c r="K16">
-        <v>0</v>
-      </c>
-      <c r="L16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <v>0</v>
-      </c>
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-      <c r="D17">
-        <v>0</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>1800</v>
-      </c>
-      <c r="I17">
-        <v>2020</v>
-      </c>
-      <c r="J17">
-        <v>156</v>
-      </c>
-      <c r="K17">
-        <v>0</v>
-      </c>
-      <c r="L17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A18">
-        <v>0</v>
-      </c>
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-      <c r="D18">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <v>1800</v>
-      </c>
-      <c r="I18">
-        <v>2020</v>
-      </c>
-      <c r="J18">
-        <v>156</v>
-      </c>
-      <c r="K18">
-        <v>0</v>
-      </c>
-      <c r="L18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A19">
-        <v>0</v>
-      </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <v>1800</v>
-      </c>
-      <c r="I19">
-        <v>2020</v>
-      </c>
-      <c r="J19">
-        <v>156</v>
-      </c>
-      <c r="K19">
-        <v>0</v>
-      </c>
-      <c r="L19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A20">
-        <v>0</v>
-      </c>
-      <c r="B20">
-        <v>0</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>0</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="F20">
-        <v>57.350000000000136</v>
-      </c>
-      <c r="G20">
-        <v>57.350000000000136</v>
-      </c>
-      <c r="H20">
-        <v>1948</v>
-      </c>
-      <c r="I20">
-        <v>2168</v>
-      </c>
-      <c r="J20">
-        <v>267</v>
-      </c>
-      <c r="K20">
-        <v>114.70000000000027</v>
-      </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A21">
-        <v>0</v>
-      </c>
-      <c r="B21">
-        <v>0</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-      <c r="D21">
-        <v>0</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="F21">
-        <v>57.350000000000136</v>
-      </c>
-      <c r="G21">
-        <v>57.350000000000136</v>
-      </c>
-      <c r="H21">
-        <v>1948</v>
-      </c>
-      <c r="I21">
-        <v>2168</v>
-      </c>
-      <c r="J21">
-        <v>267</v>
-      </c>
-      <c r="K21">
-        <v>114.70000000000027</v>
-      </c>
-      <c r="L21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A22">
-        <v>0</v>
-      </c>
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <v>1800</v>
-      </c>
-      <c r="I22">
-        <v>2020</v>
-      </c>
-      <c r="J22">
-        <v>156</v>
-      </c>
-      <c r="K22">
-        <v>0</v>
-      </c>
-      <c r="L22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A23">
-        <v>0</v>
-      </c>
-      <c r="B23">
-        <v>0</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-      <c r="D23">
-        <v>0</v>
-      </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="F23">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="H23">
-        <v>1800</v>
-      </c>
-      <c r="I23">
-        <v>2020</v>
-      </c>
-      <c r="J23">
-        <v>156</v>
-      </c>
-      <c r="K23">
-        <v>0</v>
-      </c>
-      <c r="L23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A24">
-        <v>0</v>
-      </c>
-      <c r="B24">
-        <v>0</v>
-      </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-      <c r="G24">
-        <v>0</v>
-      </c>
-      <c r="H24">
-        <v>1800</v>
-      </c>
-      <c r="I24">
-        <v>2020</v>
-      </c>
-      <c r="J24">
-        <v>156</v>
-      </c>
-      <c r="K24">
-        <v>0</v>
-      </c>
-      <c r="L24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A25">
-        <v>0</v>
-      </c>
-      <c r="B25">
-        <v>0</v>
-      </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-      <c r="G25">
-        <v>0</v>
-      </c>
-      <c r="H25">
-        <v>1592</v>
-      </c>
-      <c r="I25">
-        <v>1812</v>
-      </c>
-      <c r="J25">
-        <v>0</v>
-      </c>
-      <c r="K25">
-        <v>0</v>
-      </c>
-      <c r="L25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A27" s="1">
-        <f>SUM(A2:A25)</f>
-        <v>0</v>
-      </c>
-      <c r="B27" s="1">
-        <f t="shared" ref="B27:L27" si="0">SUM(B2:B25)</f>
-        <v>0</v>
-      </c>
-      <c r="C27" s="1">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
+        <f>A2</f>
+        <v>0</v>
+      </c>
+      <c r="B3" s="2">
+        <f>ROUND(B2,2)</f>
+        <v>0</v>
+      </c>
+      <c r="C3" s="2">
+        <f t="shared" ref="C3:M3" si="0">ROUND(C2,2)</f>
+        <v>0</v>
+      </c>
+      <c r="D3" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="D27" s="1">
+      <c r="E3" s="2">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E27" s="1">
+      <c r="F3" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F27" s="1">
+        <v>229.4</v>
+      </c>
+      <c r="G3" s="2">
         <f t="shared" si="0"/>
-        <v>229.40000000000055</v>
-      </c>
-      <c r="G27" s="1">
-        <f t="shared" si="0"/>
-        <v>229.40000000000055</v>
-      </c>
-      <c r="H27" s="1">
+        <v>229.4</v>
+      </c>
+      <c r="H3" s="2">
         <f t="shared" si="0"/>
         <v>42960</v>
       </c>
-      <c r="I27" s="1">
+      <c r="I3" s="2">
         <f t="shared" si="0"/>
         <v>48240</v>
       </c>
-      <c r="J27" s="1">
+      <c r="J3" s="2">
         <f t="shared" si="0"/>
         <v>3564</v>
       </c>
-      <c r="K27" s="1">
+      <c r="K3" s="2">
         <f t="shared" si="0"/>
-        <v>458.80000000000109</v>
-      </c>
-      <c r="L27" s="1">
+        <v>458.8</v>
+      </c>
+      <c r="L3" s="2">
         <f t="shared" si="0"/>
-        <v>-14.800000000000068</v>
+        <v>-14.8</v>
+      </c>
+      <c r="M3" s="1">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="str">
+        <f>A3&amp;","&amp;B3</f>
+        <v>0,0</v>
+      </c>
+      <c r="C4" s="1" t="str">
+        <f>B4&amp;","&amp;C3</f>
+        <v>0,0,0</v>
+      </c>
+      <c r="D4" s="1" t="str">
+        <f t="shared" ref="D4" si="1">C4&amp;","&amp;D3</f>
+        <v>0,0,0,0</v>
+      </c>
+      <c r="E4" s="1" t="str">
+        <f t="shared" ref="E4" si="2">D4&amp;","&amp;E3</f>
+        <v>0,0,0,0,0</v>
+      </c>
+      <c r="F4" s="1" t="str">
+        <f t="shared" ref="F4" si="3">E4&amp;","&amp;F3</f>
+        <v>0,0,0,0,0,229.4</v>
+      </c>
+      <c r="G4" s="1" t="str">
+        <f t="shared" ref="G4" si="4">F4&amp;","&amp;G3</f>
+        <v>0,0,0,0,0,229.4,229.4</v>
+      </c>
+      <c r="H4" s="1" t="str">
+        <f t="shared" ref="H4" si="5">G4&amp;","&amp;H3</f>
+        <v>0,0,0,0,0,229.4,229.4,42960</v>
+      </c>
+      <c r="I4" s="1" t="str">
+        <f t="shared" ref="I4" si="6">H4&amp;","&amp;I3</f>
+        <v>0,0,0,0,0,229.4,229.4,42960,48240</v>
+      </c>
+      <c r="J4" s="1" t="str">
+        <f t="shared" ref="J4" si="7">I4&amp;","&amp;J3</f>
+        <v>0,0,0,0,0,229.4,229.4,42960,48240,3564</v>
+      </c>
+      <c r="K4" s="1" t="str">
+        <f t="shared" ref="K4" si="8">J4&amp;","&amp;K3</f>
+        <v>0,0,0,0,0,229.4,229.4,42960,48240,3564,458.8</v>
+      </c>
+      <c r="L4" s="1" t="str">
+        <f>K4&amp;","&amp;L3</f>
+        <v>0,0,0,0,0,229.4,229.4,42960,48240,3564,458.8,-14.8</v>
+      </c>
+      <c r="M4" s="1" t="str">
+        <f>"["&amp;L4&amp;"]"</f>
+        <v>[0,0,0,0,0,229.4,229.4,42960,48240,3564,458.8,-14.8]</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21729D5A-FAAF-40C7-8FE8-A3EC19249BB8}">
-  <dimension ref="A1:F25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5CDEF319-98E5-44A3-8372-55829D2B15FD}">
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="A3" sqref="A3:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -2375,493 +1549,99 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2">
-        <v>0</v>
+        <v>32748.138651658672</v>
       </c>
       <c r="B2">
-        <v>24.302036340000004</v>
+        <v>29145.302839771666</v>
       </c>
       <c r="C2">
-        <v>48.812954433599998</v>
+        <v>1772.2064520913002</v>
       </c>
       <c r="D2">
-        <v>100.3301632352</v>
+        <v>3796.5983979345997</v>
       </c>
       <c r="E2">
-        <v>252.485360466</v>
+        <v>9109.3903953575009</v>
       </c>
       <c r="F2">
-        <v>111.8917538004</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>1385.7060656280023</v>
-      </c>
-      <c r="C3">
-        <v>57.422068179999997</v>
-      </c>
-      <c r="D3">
-        <v>113.54989400319998</v>
-      </c>
-      <c r="E3">
-        <v>272.51056128999994</v>
-      </c>
-      <c r="F3">
-        <v>177.7118108988</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <v>254.38532400000014</v>
-      </c>
-      <c r="C4">
-        <v>71.440061499999985</v>
-      </c>
-      <c r="D4">
-        <v>134.7802006</v>
-      </c>
-      <c r="E4">
-        <v>320.69119649999999</v>
-      </c>
-      <c r="F4">
-        <v>200.7483843</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5">
-        <v>0</v>
-      </c>
-      <c r="B5">
-        <v>540.44294271599983</v>
-      </c>
-      <c r="C5">
-        <v>83.933941190399992</v>
-      </c>
-      <c r="D5">
-        <v>140.61412697759999</v>
-      </c>
-      <c r="E5">
-        <v>376.00750689399996</v>
-      </c>
-      <c r="F5">
-        <v>243.38020736400003</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6">
-        <v>33.293499000000111</v>
-      </c>
-      <c r="B6">
-        <v>682.61210400000004</v>
-      </c>
-      <c r="C6">
-        <v>80.471868000000001</v>
-      </c>
-      <c r="D6">
-        <v>165.3032632</v>
-      </c>
-      <c r="E6">
-        <v>360.07600000000002</v>
-      </c>
-      <c r="F6">
-        <v>242.23436669999998</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7">
-        <v>510.58502699999991</v>
-      </c>
-      <c r="B7">
-        <v>466.68736499999994</v>
-      </c>
-      <c r="C7">
-        <v>78.511441000000005</v>
-      </c>
-      <c r="D7">
-        <v>161.82756560000001</v>
-      </c>
-      <c r="E7">
-        <v>361.59037849999999</v>
-      </c>
-      <c r="F7">
-        <v>232.8334284</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8">
-        <v>734.03149669200013</v>
-      </c>
-      <c r="B8">
-        <v>1002.7516805212038</v>
-      </c>
-      <c r="C8">
-        <v>74.463756712399999</v>
-      </c>
-      <c r="D8">
-        <v>168.24320778719999</v>
-      </c>
-      <c r="E8">
-        <v>402.02099732400001</v>
-      </c>
-      <c r="F8">
-        <v>242.38726096319999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9">
-        <v>2243.5342597079998</v>
-      </c>
-      <c r="B9">
-        <v>1000.3319299800002</v>
-      </c>
-      <c r="C9">
-        <v>81.684608442400005</v>
-      </c>
-      <c r="D9">
-        <v>179.68655155359997</v>
-      </c>
-      <c r="E9">
-        <v>417.23076440599993</v>
-      </c>
-      <c r="F9">
-        <v>259.27586308679997</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10">
-        <v>998.8227149999999</v>
-      </c>
-      <c r="B10">
-        <v>701.89711731600005</v>
-      </c>
-      <c r="C10">
-        <v>90.80771760639999</v>
-      </c>
-      <c r="D10">
-        <v>194.9545719784</v>
-      </c>
-      <c r="E10">
-        <v>396.86900932000003</v>
-      </c>
-      <c r="F10">
-        <v>262.82778486479998</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11">
-        <v>1671.8715175911987</v>
-      </c>
-      <c r="B11">
-        <v>1625.6903885880001</v>
-      </c>
-      <c r="C11">
-        <v>87.650746610400006</v>
-      </c>
-      <c r="D11">
-        <v>187.27110335360001</v>
-      </c>
-      <c r="E11">
-        <v>393.61740198199999</v>
-      </c>
-      <c r="F11">
-        <v>237.1648418748</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12">
-        <v>1056.2410475279999</v>
-      </c>
-      <c r="B12">
-        <v>875.42041633945894</v>
-      </c>
-      <c r="C12">
-        <v>81.475215942800006</v>
-      </c>
-      <c r="D12">
-        <v>196.99370944559999</v>
-      </c>
-      <c r="E12">
-        <v>430.50372479600003</v>
-      </c>
-      <c r="F12">
-        <v>232.605986304</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13">
-        <v>2049.3724641991998</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>67.468973680800005</v>
-      </c>
-      <c r="D13">
-        <v>173.08881551919998</v>
-      </c>
-      <c r="E13">
-        <v>406.48333094799995</v>
-      </c>
-      <c r="F13">
-        <v>241.40161565279999</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14">
-        <v>2530.9593270720002</v>
-      </c>
-      <c r="B14">
-        <v>462.12910395300008</v>
-      </c>
-      <c r="C14">
-        <v>68.222798295300009</v>
-      </c>
-      <c r="D14">
-        <v>166.79591181000001</v>
-      </c>
-      <c r="E14">
-        <v>390.2669941995</v>
-      </c>
-      <c r="F14">
-        <v>242.88705592470001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15">
-        <v>2392.2628180110005</v>
-      </c>
-      <c r="B15">
-        <v>1611.022135041</v>
-      </c>
-      <c r="C15">
-        <v>74.858283294299994</v>
-      </c>
-      <c r="D15">
-        <v>158.00428238760003</v>
-      </c>
-      <c r="E15">
-        <v>407.02367786849999</v>
-      </c>
-      <c r="F15">
-        <v>210.2187929886</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16">
-        <v>2019.129003836269</v>
-      </c>
-      <c r="B16">
-        <v>1862.855601924</v>
-      </c>
-      <c r="C16">
-        <v>71.699423992000007</v>
-      </c>
-      <c r="D16">
-        <v>149.68102399439999</v>
-      </c>
-      <c r="E16">
-        <v>391.75955052</v>
-      </c>
-      <c r="F16">
-        <v>153.69130396079998</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17">
-        <v>2336.1035016599999</v>
-      </c>
-      <c r="B17">
-        <v>72.895331279999724</v>
-      </c>
-      <c r="C17">
-        <v>69.0141358164</v>
-      </c>
-      <c r="D17">
-        <v>153.03711607760002</v>
-      </c>
-      <c r="E17">
-        <v>375.63208912199997</v>
-      </c>
-      <c r="F17">
-        <v>172.03733741639999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18">
-        <v>2137.6195277520001</v>
-      </c>
-      <c r="B18">
-        <v>1357.4608634500014</v>
-      </c>
-      <c r="C18">
-        <v>68.711391361599993</v>
-      </c>
-      <c r="D18">
-        <v>154.1370470912</v>
-      </c>
-      <c r="E18">
-        <v>367.40801968400001</v>
-      </c>
-      <c r="F18">
-        <v>152.22435066119999</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19">
-        <v>2056.0861203240001</v>
-      </c>
-      <c r="B19">
-        <v>2275.7208708839999</v>
-      </c>
-      <c r="C19">
-        <v>70.828895149200008</v>
-      </c>
-      <c r="D19">
-        <v>155.0712731664</v>
-      </c>
-      <c r="E19">
-        <v>375.93832316599998</v>
-      </c>
-      <c r="F19">
-        <v>142.06418968079998</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20">
-        <v>2382.4805281200001</v>
-      </c>
-      <c r="B20">
-        <v>2545.9547949990006</v>
-      </c>
-      <c r="C20">
-        <v>53.445205291500002</v>
-      </c>
-      <c r="D20">
-        <v>170.6165415504</v>
-      </c>
-      <c r="E20">
-        <v>361.33387047450009</v>
-      </c>
-      <c r="F20">
-        <v>180.88979837939999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21">
-        <v>2349.2134348650002</v>
-      </c>
-      <c r="B21">
-        <v>2651.3372084760003</v>
-      </c>
-      <c r="C21">
-        <v>65.796251578200014</v>
-      </c>
-      <c r="D21">
-        <v>167.27073737219999</v>
-      </c>
-      <c r="E21">
-        <v>403.64475534899998</v>
-      </c>
-      <c r="F21">
-        <v>214.23567207240004</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22">
-        <v>2308.575626196</v>
-      </c>
-      <c r="B22">
-        <v>2567.2921315199997</v>
-      </c>
-      <c r="C22">
-        <v>72.920152167999987</v>
-      </c>
-      <c r="D22">
-        <v>154.14461980799999</v>
-      </c>
-      <c r="E22">
-        <v>429.65724246400003</v>
-      </c>
-      <c r="F22">
-        <v>214.53319427879998</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23">
-        <v>415.21634693999999</v>
-      </c>
-      <c r="B23">
-        <v>2462.430187512</v>
-      </c>
-      <c r="C23">
-        <v>85.899096231599998</v>
-      </c>
-      <c r="D23">
-        <v>163.00634884159999</v>
-      </c>
-      <c r="E23">
-        <v>399.54399073599996</v>
-      </c>
-      <c r="F23">
-        <v>202.16246517240003</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24">
-        <v>1954.8073661639999</v>
-      </c>
-      <c r="B24">
-        <v>1924.1028473040001</v>
-      </c>
-      <c r="C24">
-        <v>85.881460713999985</v>
-      </c>
-      <c r="D24">
-        <v>159.53442798159998</v>
-      </c>
-      <c r="E24">
-        <v>421.97897534800001</v>
-      </c>
-      <c r="F24">
-        <v>100.83729887639998</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25">
-        <v>567.93302399999993</v>
-      </c>
-      <c r="B25">
-        <v>791.87439299999994</v>
-      </c>
-      <c r="C25">
-        <v>80.786004899999995</v>
-      </c>
-      <c r="D25">
-        <v>128.65589459999998</v>
-      </c>
-      <c r="E25">
-        <v>395.11667399999999</v>
-      </c>
-      <c r="F25">
-        <v>48.065860200000003</v>
+        <v>4718.3106238214996</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
+        <f>A2</f>
+        <v>32748.138651658672</v>
+      </c>
+      <c r="B3" s="2">
+        <f>ROUND(B2,2)</f>
+        <v>29145.3</v>
+      </c>
+      <c r="C3" s="2">
+        <f t="shared" ref="C3:M3" si="0">ROUND(C2,2)</f>
+        <v>1772.21</v>
+      </c>
+      <c r="D3" s="2">
+        <f t="shared" si="0"/>
+        <v>3796.6</v>
+      </c>
+      <c r="E3" s="2">
+        <f t="shared" si="0"/>
+        <v>9109.39</v>
+      </c>
+      <c r="F3" s="2">
+        <f t="shared" si="0"/>
+        <v>4718.3100000000004</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="str">
+        <f>A3&amp;","&amp;B3</f>
+        <v>32748.1386516587,29145.3</v>
+      </c>
+      <c r="C4" s="1" t="str">
+        <f>B4&amp;","&amp;C3</f>
+        <v>32748.1386516587,29145.3,1772.21</v>
+      </c>
+      <c r="D4" s="1" t="str">
+        <f t="shared" ref="D4:K4" si="1">C4&amp;","&amp;D3</f>
+        <v>32748.1386516587,29145.3,1772.21,3796.6</v>
+      </c>
+      <c r="E4" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>32748.1386516587,29145.3,1772.21,3796.6,9109.39</v>
+      </c>
+      <c r="F4" s="1" t="str">
+        <f t="shared" si="1"/>
+        <v>32748.1386516587,29145.3,1772.21,3796.6,9109.39,4718.31</v>
+      </c>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1" t="str">
+        <f>"["&amp;F4&amp;"]"</f>
+        <v>[32748.1386516587,29145.3,1772.21,3796.6,9109.39,4718.31]</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DECBBDCB-F374-4D19-ACD4-46256F8A15F2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B34A915-06DE-439C-A27B-F3C33B5EA90C}">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2918,7 +1698,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D376BD51-5212-408C-B01F-2E5A50462DEF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC16084D-EB8B-4B7A-A93D-4F6BCDEDD88A}">
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3206,7 +1986,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2576DD9-3A0E-433A-8050-260C7B30451A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE44B617-0C14-49D4-9F38-32932591EEED}">
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3494,7 +2274,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CD3CDE3-F1B8-4756-8F84-64C6374A6D17}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7A89DD4-91BD-4F2E-A74F-E22D14914844}">
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3782,7 +2562,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36599E27-47EA-435A-8CFE-BE229FD3A2C7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDCE40EF-CA5D-4D8D-83F9-C1D2A911BDD9}">
   <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -4745,7 +3525,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DD4977C-3BFE-4C1B-AD1D-13F9FB59A381}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9421DC1-E95A-403A-B216-ACA0CBE9B66D}">
   <dimension ref="A1:Q25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -6083,7 +4863,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9B3F32F-0728-4573-9448-0C5062A33804}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27CEAD9B-6BBD-4082-934B-3293FABBD00A}">
   <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -6596,7 +5376,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{098516A3-2341-4F8B-A6CA-5839DED59227}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{39C89E50-90BD-47A7-8A4B-BE6DE47E55F0}">
   <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>